<commit_message>
fix: vis dice sunarp
</commit_message>
<xml_diff>
--- a/backend/docs/VIS-PLA.xlsx
+++ b/backend/docs/VIS-PLA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\planosperu-app\backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C726DC-9C85-4E1D-B9C5-7CBD6217999A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D0D6C8-AD9C-4F28-A066-7EEAF900869E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{A2F3C56B-C265-481F-806E-CD3616F017BF}"/>
   </bookViews>
@@ -260,9 +260,6 @@
     <t>para el ingreso a Municipio</t>
   </si>
   <si>
-    <t>entidad Sunarp hasta su aceptacion y Aprobacion</t>
-  </si>
-  <si>
     <t xml:space="preserve">2.2 CD - Grabación Digital del Proyecto </t>
   </si>
   <si>
@@ -333,6 +330,9 @@
   </si>
   <si>
     <t>Ing. Aguirre Alanya Luis Antonio CIP: 323997 CIV: 022178VCZRIX</t>
+  </si>
+  <si>
+    <t>entidad Municipal hasta su aceptacion y Aprobacion</t>
   </si>
 </sst>
 </file>
@@ -838,20 +838,74 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
@@ -861,6 +915,207 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -909,275 +1164,20 @@
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2147,8 +2147,8 @@
   </sheetPr>
   <dimension ref="A3:H79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A49" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60:G60"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A42" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50:G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2170,86 +2170,86 @@
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
+      <c r="E4" s="137"/>
+      <c r="F4" s="137"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="138" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
+      <c r="E5" s="138"/>
+      <c r="F5" s="138"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="139" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
+      <c r="E6" s="139"/>
+      <c r="F6" s="139"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="D7" s="140" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
+      <c r="E7" s="140"/>
+      <c r="F7" s="140"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
+      <c r="A8" s="141"/>
+      <c r="B8" s="141"/>
+      <c r="C8" s="141"/>
+      <c r="D8" s="141"/>
+      <c r="E8" s="141"/>
+      <c r="F8" s="141"/>
+      <c r="G8" s="141"/>
+      <c r="H8" s="141"/>
     </row>
     <row r="9" spans="1:8" s="5" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="136" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
+      <c r="C9" s="136"/>
+      <c r="D9" s="136"/>
+      <c r="E9" s="136"/>
+      <c r="F9" s="136"/>
+      <c r="G9" s="136"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
+      <c r="B10" s="136"/>
+      <c r="C10" s="136"/>
+      <c r="D10" s="136"/>
+      <c r="E10" s="136"/>
+      <c r="F10" s="136"/>
+      <c r="G10" s="136"/>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="124" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
+      <c r="C11" s="124"/>
+      <c r="D11" s="124"/>
+      <c r="E11" s="124"/>
       <c r="F11" s="8" t="s">
         <v>12</v>
       </c>
@@ -2258,22 +2258,22 @@
     </row>
     <row r="12" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
+      <c r="B12" s="124"/>
+      <c r="C12" s="124"/>
+      <c r="D12" s="124"/>
+      <c r="E12" s="124"/>
+      <c r="F12" s="124"/>
+      <c r="G12" s="124"/>
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
-      <c r="B13" s="54"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
+      <c r="B13" s="124"/>
+      <c r="C13" s="124"/>
+      <c r="D13" s="124"/>
+      <c r="E13" s="124"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="124"/>
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -2298,10 +2298,10 @@
       <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
+      <c r="B15" s="124"/>
+      <c r="C15" s="124"/>
+      <c r="D15" s="124"/>
+      <c r="E15" s="124"/>
       <c r="F15" s="13" t="s">
         <v>18</v>
       </c>
@@ -2310,10 +2310,10 @@
     </row>
     <row r="16" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
+      <c r="B16" s="125"/>
+      <c r="C16" s="125"/>
+      <c r="D16" s="125"/>
+      <c r="E16" s="125"/>
       <c r="F16" s="13" t="s">
         <v>19</v>
       </c>
@@ -2324,10 +2324,10 @@
       <c r="A17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="54"/>
+      <c r="C17" s="124"/>
       <c r="D17" s="18" t="s">
         <v>22</v>
       </c>
@@ -2341,167 +2341,167 @@
     </row>
     <row r="18" spans="1:8" s="11" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
+      <c r="B18" s="126"/>
+      <c r="C18" s="126"/>
+      <c r="D18" s="126"/>
+      <c r="E18" s="126"/>
+      <c r="F18" s="126"/>
+      <c r="G18" s="126"/>
       <c r="H18" s="20"/>
     </row>
     <row r="19" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="58"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
+      <c r="C19" s="128"/>
+      <c r="D19" s="129"/>
+      <c r="E19" s="130"/>
+      <c r="F19" s="130"/>
+      <c r="G19" s="130"/>
       <c r="H19" s="22"/>
     </row>
     <row r="20" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="131" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="62"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="64" t="s">
+      <c r="C20" s="132"/>
+      <c r="D20" s="133"/>
+      <c r="E20" s="134" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="64"/>
-      <c r="G20" s="65"/>
+      <c r="F20" s="134"/>
+      <c r="G20" s="135"/>
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="52"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="52" t="s">
+      <c r="C21" s="65"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="52"/>
-      <c r="G21" s="53"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="66"/>
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
-      <c r="B22" s="66" t="s">
+      <c r="B22" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="69"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="122"/>
+      <c r="F22" s="122"/>
+      <c r="G22" s="123"/>
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="70" t="s">
+      <c r="C23" s="65"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="119" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="71"/>
-      <c r="G23" s="72"/>
+      <c r="F23" s="120"/>
+      <c r="G23" s="121"/>
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="52"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="51" t="s">
+      <c r="C24" s="65"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="52"/>
-      <c r="G24" s="53"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="66"/>
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
-      <c r="B25" s="51" t="s">
+      <c r="B25" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="52"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="51" t="s">
+      <c r="C25" s="65"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="52"/>
-      <c r="G25" s="53"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="66"/>
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
-      <c r="B26" s="70" t="s">
+      <c r="B26" s="119" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="71"/>
-      <c r="D26" s="72"/>
-      <c r="E26" s="51" t="s">
+      <c r="C26" s="120"/>
+      <c r="D26" s="121"/>
+      <c r="E26" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="52"/>
-      <c r="G26" s="53"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="66"/>
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
-      <c r="B27" s="73" t="s">
+      <c r="B27" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="74"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="51" t="s">
+      <c r="C27" s="82"/>
+      <c r="D27" s="83"/>
+      <c r="E27" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="52"/>
-      <c r="G27" s="53"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="66"/>
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25"/>
-      <c r="B28" s="73" t="s">
+      <c r="B28" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="74"/>
-      <c r="D28" s="75"/>
-      <c r="E28" s="82"/>
-      <c r="F28" s="83"/>
-      <c r="G28" s="84"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="83"/>
+      <c r="E28" s="108"/>
+      <c r="F28" s="109"/>
+      <c r="G28" s="110"/>
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
-      <c r="B29" s="66" t="s">
+      <c r="B29" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="85"/>
-      <c r="F29" s="85"/>
-      <c r="G29" s="86"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="111"/>
+      <c r="F29" s="111"/>
+      <c r="G29" s="112"/>
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="29"/>
-      <c r="B30" s="87" t="s">
+      <c r="B30" s="113" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="88"/>
-      <c r="D30" s="89"/>
+      <c r="C30" s="114"/>
+      <c r="D30" s="115"/>
       <c r="E30" s="30" t="s">
         <v>42</v>
       </c>
@@ -2511,11 +2511,11 @@
     </row>
     <row r="31" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="29"/>
-      <c r="B31" s="73" t="s">
+      <c r="B31" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="74"/>
-      <c r="D31" s="75"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="83"/>
       <c r="E31" s="26" t="s">
         <v>44</v>
       </c>
@@ -2525,11 +2525,11 @@
     </row>
     <row r="32" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="33"/>
-      <c r="B32" s="90" t="s">
+      <c r="B32" s="116" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="91"/>
-      <c r="D32" s="92"/>
+      <c r="C32" s="117"/>
+      <c r="D32" s="118"/>
       <c r="E32" s="26" t="s">
         <v>46</v>
       </c>
@@ -2539,89 +2539,89 @@
     </row>
     <row r="33" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
-      <c r="B33" s="90"/>
-      <c r="C33" s="91"/>
-      <c r="D33" s="92"/>
-      <c r="E33" s="73" t="s">
+      <c r="B33" s="116"/>
+      <c r="C33" s="117"/>
+      <c r="D33" s="118"/>
+      <c r="E33" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="74"/>
-      <c r="G33" s="75"/>
+      <c r="F33" s="82"/>
+      <c r="G33" s="83"/>
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
-      <c r="B34" s="73" t="s">
+      <c r="B34" s="81" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="74"/>
-      <c r="D34" s="75"/>
-      <c r="E34" s="73" t="s">
+      <c r="C34" s="82"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="F34" s="74"/>
-      <c r="G34" s="75"/>
+      <c r="F34" s="82"/>
+      <c r="G34" s="83"/>
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
-      <c r="B35" s="90" t="s">
+      <c r="B35" s="116" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="91"/>
-      <c r="D35" s="92"/>
-      <c r="E35" s="73" t="s">
+      <c r="C35" s="117"/>
+      <c r="D35" s="118"/>
+      <c r="E35" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="F35" s="74"/>
-      <c r="G35" s="75"/>
+      <c r="F35" s="82"/>
+      <c r="G35" s="83"/>
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
-      <c r="B36" s="90"/>
-      <c r="C36" s="91"/>
-      <c r="D36" s="92"/>
-      <c r="E36" s="93" t="s">
+      <c r="B36" s="116"/>
+      <c r="C36" s="117"/>
+      <c r="D36" s="118"/>
+      <c r="E36" s="87" t="s">
         <v>52</v>
       </c>
-      <c r="F36" s="94"/>
-      <c r="G36" s="95"/>
+      <c r="F36" s="88"/>
+      <c r="G36" s="89"/>
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
-      <c r="B37" s="76" t="s">
+      <c r="B37" s="105" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="77"/>
-      <c r="D37" s="78"/>
-      <c r="E37" s="79" t="s">
+      <c r="C37" s="106"/>
+      <c r="D37" s="107"/>
+      <c r="E37" s="102" t="s">
         <v>54</v>
       </c>
-      <c r="F37" s="80"/>
-      <c r="G37" s="81"/>
+      <c r="F37" s="103"/>
+      <c r="G37" s="104"/>
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
-      <c r="B38" s="73" t="s">
+      <c r="B38" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="74"/>
-      <c r="D38" s="75"/>
-      <c r="E38" s="79"/>
-      <c r="F38" s="80"/>
-      <c r="G38" s="81"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="83"/>
+      <c r="E38" s="102"/>
+      <c r="F38" s="103"/>
+      <c r="G38" s="104"/>
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
-      <c r="B39" s="93" t="s">
+      <c r="B39" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="94"/>
-      <c r="D39" s="95"/>
+      <c r="C39" s="88"/>
+      <c r="D39" s="89"/>
       <c r="E39" s="96" t="s">
         <v>57</v>
       </c>
@@ -2631,11 +2631,11 @@
     </row>
     <row r="40" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
-      <c r="B40" s="73" t="s">
+      <c r="B40" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="C40" s="74"/>
-      <c r="D40" s="75"/>
+      <c r="C40" s="82"/>
+      <c r="D40" s="83"/>
       <c r="E40" s="99" t="s">
         <v>59</v>
       </c>
@@ -2645,208 +2645,208 @@
     </row>
     <row r="41" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
-      <c r="B41" s="73" t="s">
+      <c r="B41" s="81" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="74"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="79" t="s">
+      <c r="C41" s="82"/>
+      <c r="D41" s="83"/>
+      <c r="E41" s="102" t="s">
         <v>61</v>
       </c>
-      <c r="F41" s="80"/>
-      <c r="G41" s="81"/>
+      <c r="F41" s="103"/>
+      <c r="G41" s="104"/>
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
-      <c r="B42" s="73" t="s">
+      <c r="B42" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="74"/>
-      <c r="D42" s="75"/>
-      <c r="E42" s="79"/>
-      <c r="F42" s="80"/>
-      <c r="G42" s="81"/>
+      <c r="C42" s="82"/>
+      <c r="D42" s="83"/>
+      <c r="E42" s="102"/>
+      <c r="F42" s="103"/>
+      <c r="G42" s="104"/>
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
-      <c r="B43" s="73" t="s">
+      <c r="B43" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="C43" s="74"/>
-      <c r="D43" s="75"/>
-      <c r="E43" s="102" t="s">
+      <c r="C43" s="82"/>
+      <c r="D43" s="83"/>
+      <c r="E43" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="F43" s="103"/>
-      <c r="G43" s="104"/>
+      <c r="F43" s="85"/>
+      <c r="G43" s="86"/>
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
-      <c r="B44" s="93" t="s">
+      <c r="B44" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="C44" s="94"/>
-      <c r="D44" s="95"/>
-      <c r="E44" s="105"/>
-      <c r="F44" s="106"/>
-      <c r="G44" s="107"/>
+      <c r="C44" s="88"/>
+      <c r="D44" s="89"/>
+      <c r="E44" s="90"/>
+      <c r="F44" s="91"/>
+      <c r="G44" s="92"/>
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
-      <c r="B45" s="73" t="s">
+      <c r="B45" s="81" t="s">
         <v>66</v>
       </c>
-      <c r="C45" s="74"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="108"/>
-      <c r="F45" s="109"/>
-      <c r="G45" s="110"/>
+      <c r="C45" s="82"/>
+      <c r="D45" s="83"/>
+      <c r="E45" s="93"/>
+      <c r="F45" s="94"/>
+      <c r="G45" s="95"/>
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="66" t="s">
+      <c r="B46" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="67"/>
-      <c r="D46" s="67"/>
-      <c r="E46" s="112"/>
-      <c r="F46" s="112"/>
-      <c r="G46" s="113"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="58"/>
+      <c r="E46" s="59"/>
+      <c r="F46" s="59"/>
+      <c r="G46" s="60"/>
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
-      <c r="B47" s="114" t="s">
+      <c r="B47" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C47" s="115"/>
-      <c r="D47" s="116"/>
-      <c r="E47" s="51" t="s">
+      <c r="C47" s="62"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="F47" s="52"/>
-      <c r="G47" s="53"/>
+      <c r="F47" s="65"/>
+      <c r="G47" s="66"/>
       <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
-      <c r="B48" s="117" t="s">
+      <c r="B48" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="C48" s="118"/>
-      <c r="D48" s="119"/>
-      <c r="E48" s="117" t="s">
+      <c r="C48" s="68"/>
+      <c r="D48" s="69"/>
+      <c r="E48" s="67" t="s">
         <v>71</v>
       </c>
-      <c r="F48" s="118"/>
-      <c r="G48" s="119"/>
+      <c r="F48" s="68"/>
+      <c r="G48" s="69"/>
       <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
-      <c r="B49" s="117" t="s">
+      <c r="B49" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="C49" s="118"/>
-      <c r="D49" s="119"/>
-      <c r="E49" s="120" t="s">
-        <v>73</v>
-      </c>
-      <c r="F49" s="121"/>
-      <c r="G49" s="122"/>
+      <c r="C49" s="68"/>
+      <c r="D49" s="69"/>
+      <c r="E49" s="70" t="s">
+        <v>97</v>
+      </c>
+      <c r="F49" s="71"/>
+      <c r="G49" s="72"/>
       <c r="H49" s="10"/>
     </row>
     <row r="50" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
-      <c r="B50" s="123" t="s">
-        <v>74</v>
-      </c>
-      <c r="C50" s="124"/>
-      <c r="D50" s="125"/>
-      <c r="E50" s="126"/>
-      <c r="F50" s="127"/>
-      <c r="G50" s="128"/>
+      <c r="B50" s="73" t="s">
+        <v>73</v>
+      </c>
+      <c r="C50" s="74"/>
+      <c r="D50" s="75"/>
+      <c r="E50" s="76"/>
+      <c r="F50" s="77"/>
+      <c r="G50" s="78"/>
       <c r="H50" s="10"/>
     </row>
     <row r="51" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
-      <c r="B51" s="129"/>
-      <c r="C51" s="129"/>
-      <c r="D51" s="129"/>
-      <c r="E51" s="129"/>
-      <c r="F51" s="129"/>
-      <c r="G51" s="129"/>
+      <c r="B51" s="79"/>
+      <c r="C51" s="79"/>
+      <c r="D51" s="79"/>
+      <c r="E51" s="79"/>
+      <c r="F51" s="79"/>
+      <c r="G51" s="79"/>
       <c r="H51" s="10"/>
     </row>
     <row r="52" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="C52" s="130"/>
-      <c r="D52" s="130"/>
-      <c r="E52" s="130"/>
-      <c r="F52" s="130"/>
-      <c r="G52" s="130"/>
+        <v>74</v>
+      </c>
+      <c r="C52" s="80"/>
+      <c r="D52" s="80"/>
+      <c r="E52" s="80"/>
+      <c r="F52" s="80"/>
+      <c r="G52" s="80"/>
       <c r="H52" s="10"/>
     </row>
     <row r="53" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
-      <c r="B53" s="111"/>
-      <c r="C53" s="111"/>
-      <c r="D53" s="111"/>
-      <c r="E53" s="111"/>
-      <c r="F53" s="111"/>
-      <c r="G53" s="111"/>
+      <c r="B53" s="56"/>
+      <c r="C53" s="56"/>
+      <c r="D53" s="56"/>
+      <c r="E53" s="56"/>
+      <c r="F53" s="56"/>
+      <c r="G53" s="56"/>
       <c r="H53" s="10"/>
     </row>
     <row r="54" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
-      <c r="B54" s="111"/>
-      <c r="C54" s="111"/>
-      <c r="D54" s="111"/>
-      <c r="E54" s="111"/>
-      <c r="F54" s="111"/>
-      <c r="G54" s="111"/>
+      <c r="B54" s="56"/>
+      <c r="C54" s="56"/>
+      <c r="D54" s="56"/>
+      <c r="E54" s="56"/>
+      <c r="F54" s="56"/>
+      <c r="G54" s="56"/>
       <c r="H54" s="10"/>
     </row>
     <row r="55" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
-      <c r="B55" s="132"/>
-      <c r="C55" s="132"/>
-      <c r="D55" s="132"/>
-      <c r="E55" s="132"/>
-      <c r="F55" s="132"/>
-      <c r="G55" s="132"/>
+      <c r="B55" s="48"/>
+      <c r="C55" s="48"/>
+      <c r="D55" s="48"/>
+      <c r="E55" s="48"/>
+      <c r="F55" s="48"/>
+      <c r="G55" s="48"/>
       <c r="H55" s="10"/>
     </row>
     <row r="56" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="21"/>
-      <c r="B56" s="133" t="s">
-        <v>76</v>
-      </c>
-      <c r="C56" s="133"/>
-      <c r="D56" s="133"/>
-      <c r="E56" s="133"/>
-      <c r="F56" s="133"/>
-      <c r="G56" s="133"/>
+      <c r="B56" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="C56" s="49"/>
+      <c r="D56" s="49"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="49"/>
+      <c r="G56" s="49"/>
       <c r="H56" s="22"/>
     </row>
     <row r="57" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="22"/>
-      <c r="B57" s="134" t="s">
-        <v>77</v>
-      </c>
-      <c r="C57" s="134"/>
+      <c r="B57" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="C57" s="50"/>
       <c r="D57" s="35">
         <v>6</v>
       </c>
       <c r="E57" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F57" s="20"/>
       <c r="G57" s="20"/>
@@ -2854,56 +2854,56 @@
     </row>
     <row r="58" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
-      <c r="B58" s="133" t="s">
-        <v>79</v>
-      </c>
-      <c r="C58" s="133"/>
-      <c r="D58" s="133"/>
-      <c r="E58" s="133"/>
-      <c r="F58" s="133"/>
-      <c r="G58" s="133"/>
+      <c r="B58" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58" s="49"/>
+      <c r="D58" s="49"/>
+      <c r="E58" s="49"/>
+      <c r="F58" s="49"/>
+      <c r="G58" s="49"/>
       <c r="H58" s="22"/>
     </row>
     <row r="59" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="22"/>
-      <c r="B59" s="135" t="s">
-        <v>80</v>
-      </c>
-      <c r="C59" s="135"/>
+      <c r="B59" s="51" t="s">
+        <v>79</v>
+      </c>
+      <c r="C59" s="51"/>
       <c r="D59" s="37">
         <f>C61+C62</f>
         <v>0</v>
       </c>
-      <c r="E59" s="136" t="s">
-        <v>81</v>
-      </c>
-      <c r="F59" s="136"/>
+      <c r="E59" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="F59" s="52"/>
       <c r="G59" s="20"/>
       <c r="H59" s="22"/>
     </row>
     <row r="60" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="21"/>
-      <c r="B60" s="133" t="s">
-        <v>82</v>
-      </c>
-      <c r="C60" s="133"/>
-      <c r="D60" s="133"/>
-      <c r="E60" s="133"/>
-      <c r="F60" s="133"/>
-      <c r="G60" s="133"/>
+      <c r="B60" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="C60" s="49"/>
+      <c r="D60" s="49"/>
+      <c r="E60" s="49"/>
+      <c r="F60" s="49"/>
+      <c r="G60" s="49"/>
       <c r="H60" s="22"/>
     </row>
     <row r="61" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="22"/>
       <c r="B61" s="36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C61" s="37"/>
-      <c r="D61" s="137" t="s">
-        <v>94</v>
-      </c>
-      <c r="E61" s="138"/>
-      <c r="F61" s="138"/>
+      <c r="D61" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="E61" s="54"/>
+      <c r="F61" s="54"/>
       <c r="G61" s="38">
         <f ca="1">E17</f>
         <v>45838</v>
@@ -2913,95 +2913,95 @@
     <row r="62" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="22"/>
       <c r="B62" s="36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C62" s="39"/>
-      <c r="D62" s="138" t="s">
-        <v>83</v>
-      </c>
-      <c r="E62" s="138"/>
-      <c r="F62" s="138"/>
+      <c r="D62" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="E62" s="54"/>
+      <c r="F62" s="54"/>
       <c r="G62" s="38">
         <f ca="1">E17+8</f>
         <v>45846</v>
       </c>
       <c r="H62" s="40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
-      <c r="B63" s="139" t="s">
-        <v>85</v>
-      </c>
-      <c r="C63" s="139"/>
-      <c r="D63" s="139"/>
-      <c r="E63" s="139"/>
-      <c r="F63" s="139"/>
-      <c r="G63" s="139"/>
+      <c r="B63" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="C63" s="55"/>
+      <c r="D63" s="55"/>
+      <c r="E63" s="55"/>
+      <c r="F63" s="55"/>
+      <c r="G63" s="55"/>
       <c r="H63" s="41"/>
     </row>
     <row r="64" spans="1:8" s="23" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B64" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="B64" s="131" t="s">
+      <c r="C64" s="47"/>
+      <c r="D64" s="47"/>
+      <c r="E64" s="47"/>
+      <c r="F64" s="47"/>
+      <c r="G64" s="47"/>
+    </row>
+    <row r="65" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C65" s="45"/>
+      <c r="D65" s="45"/>
+      <c r="E65" s="45"/>
+      <c r="F65" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="C64" s="131"/>
-      <c r="D64" s="131"/>
-      <c r="E64" s="131"/>
-      <c r="F64" s="131"/>
-      <c r="G64" s="131"/>
-    </row>
-    <row r="65" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="140" t="s">
-        <v>97</v>
-      </c>
-      <c r="C65" s="140"/>
-      <c r="D65" s="140"/>
-      <c r="E65" s="140"/>
-      <c r="F65" s="140" t="s">
+      <c r="G65" s="45"/>
+      <c r="H65" s="45"/>
+    </row>
+    <row r="66" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="G65" s="140"/>
-      <c r="H65" s="140"/>
-    </row>
-    <row r="66" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="141" t="s">
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="C66" s="141"/>
-      <c r="D66" s="141"/>
-      <c r="E66" s="141"/>
-      <c r="F66" s="140" t="s">
+      <c r="G66" s="45"/>
+      <c r="H66" s="45"/>
+    </row>
+    <row r="67" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="G66" s="140"/>
-      <c r="H66" s="140"/>
-    </row>
-    <row r="67" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="141" t="s">
+      <c r="C67" s="46"/>
+      <c r="D67" s="46"/>
+      <c r="E67" s="46"/>
+      <c r="F67" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="C67" s="141"/>
-      <c r="D67" s="141"/>
-      <c r="E67" s="141"/>
-      <c r="F67" s="140" t="s">
+      <c r="G67" s="45"/>
+      <c r="H67" s="45"/>
+    </row>
+    <row r="68" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="G67" s="140"/>
-      <c r="H67" s="140"/>
-    </row>
-    <row r="68" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="140" t="s">
-        <v>93</v>
-      </c>
-      <c r="C68" s="140"/>
-      <c r="D68" s="140"/>
-      <c r="E68" s="140"/>
-      <c r="F68" s="140"/>
-      <c r="G68" s="140"/>
+      <c r="C68" s="45"/>
+      <c r="D68" s="45"/>
+      <c r="E68" s="45"/>
+      <c r="F68" s="45"/>
+      <c r="G68" s="45"/>
     </row>
     <row r="69" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="43"/>
@@ -3029,51 +3029,37 @@
     <protectedRange algorithmName="SHA-512" hashValue="1IwEtpPovyRjspz9ti3J5udl070IPZ9gDlGmM3ZH/lFyQlLVVL2qbaMds7kHvZZkPq7VvowLV2MqpNnf8owpjQ==" saltValue="SwYyjj//I75seGLqQP0hyQ==" spinCount="100000" sqref="E37:G38 E39" name="Rango2_2"/>
   </protectedRanges>
   <mergeCells count="91">
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="B63:G63"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G42"/>
-    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B9:G10"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:G27"/>
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="E37:G38"/>
     <mergeCell ref="B38:D38"/>
@@ -3089,37 +3075,51 @@
     <mergeCell ref="B35:D36"/>
     <mergeCell ref="E35:G35"/>
     <mergeCell ref="E36:G36"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="B9:G10"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G42"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="B63:G63"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="F67:H67"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1" xr:uid="{2FC5AD4B-1AFC-41B6-9E4B-A315E4243A12}"/>

</xml_diff>